<commit_message>
Edited El Hosni Yassine xl File
added a new date...
</commit_message>
<xml_diff>
--- a/PFF-202/Stagiaires/ElHosni Yassine.xlsx
+++ b/PFF-202/Stagiaires/ElHosni Yassine.xlsx
@@ -562,7 +562,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +745,12 @@
       <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="E9" s="2">
+        <v>42865</v>
+      </c>
+      <c r="F9" s="2">
+        <v>42866</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>

<commit_message>
Edited ElHosni Yassine xl file
added some dates...
</commit_message>
<xml_diff>
--- a/PFF-202/Stagiaires/ElHosni Yassine.xlsx
+++ b/PFF-202/Stagiaires/ElHosni Yassine.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010"/>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -315,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -561,11 +561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
@@ -728,6 +728,12 @@
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E8" s="2">
+        <v>42818</v>
+      </c>
+      <c r="F8" s="2">
+        <v>42821</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -905,7 +911,7 @@
         <v>42800</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>